<commit_message>
- Updated Test Data file for Searching Dress
</commit_message>
<xml_diff>
--- a/src/test/java/testData/testData.xlsx
+++ b/src/test/java/testData/testData.xlsx
@@ -5,13 +5,33 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginTestData" sheetId="1" r:id="rId4"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
+    <sheet name="LoginTestData" sheetId="2" r:id="rId5"/>
+    <sheet name="DressSearch" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+  <si>
+    <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
+  </si>
+  <si>
+    <t>Numbers Sheet Name</t>
+  </si>
+  <si>
+    <t>Numbers Table Name</t>
+  </si>
+  <si>
+    <t>Excel Worksheet Name</t>
+  </si>
+  <si>
+    <t>LoginTestData</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
   <si>
     <t>emailAddress</t>
   </si>
@@ -23,7 +43,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="10"/>
+        <color indexed="14"/>
         <rFont val="Arial"/>
       </rPr>
       <t>vjyvgns@live.com</t>
@@ -31,6 +51,15 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>DressSearch</t>
+  </si>
+  <si>
+    <t>DressType</t>
+  </si>
+  <si>
+    <t>Summer Dress</t>
   </si>
 </sst>
 </file>
@@ -40,9 +69,19 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
@@ -52,6 +91,12 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -59,19 +104,49 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="10"/>
+      <color indexed="14"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -81,16 +156,168 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
       </bottom>
       <diagonal/>
     </border>
@@ -100,17 +327,89 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -130,8 +429,16 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff1155cc"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -330,12 +637,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -368,10 +675,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -619,12 +926,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -939,10 +1246,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1193,82 +1500,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="4" width="33.6016" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" ht="0.05" customHeight="1">
+      <c r="B3" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s" s="5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:D3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D10" location="'LoginTestData'!R1C1" tooltip="" display="LoginTestData"/>
+    <hyperlink ref="D12" location="'DressSearch'!R1C1" tooltip="" display="DressSearch"/>
+  </hyperlinks>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="5" width="14.5" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
+      <c r="A1" t="s" s="7">
+        <v>6</v>
       </c>
-      <c r="B1" t="s" s="2">
-        <v>1</v>
+      <c r="B1" t="s" s="7">
+        <v>7</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="2">
-        <v>2</v>
+      <c r="A2" t="s" s="7">
+        <v>8</v>
       </c>
-      <c r="B2" t="s" s="2">
-        <v>3</v>
+      <c r="B2" t="s" s="7">
+        <v>9</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1280,4 +1673,104 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.65" customHeight="1">
+      <c r="A1" t="s" s="16">
+        <v>11</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1">
+      <c r="A2" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" s="21"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="21"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="21"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="21"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="21"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="21"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" ht="13.3" customHeight="1">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+    </row>
+    <row r="10" ht="13" customHeight="1">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>